<commit_message>
Updated Clean_It_RawData1.ipynb and ExcelOutput
</commit_message>
<xml_diff>
--- a/ChevronDataFiles/P-16051_Raw_Data1_Cleaned.xlsx
+++ b/ChevronDataFiles/P-16051_Raw_Data1_Cleaned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Epoch</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>MBPD.2</t>
+  </si>
+  <si>
+    <t>VIB</t>
   </si>
 </sst>
 </file>
@@ -435,13 +438,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U6983"/>
+  <dimension ref="A1:V6983"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:22">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -502,8 +505,11 @@
       <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:21">
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -567,8 +573,11 @@
       <c r="U2">
         <v>88.22983182406213</v>
       </c>
-    </row>
-    <row r="3" spans="1:21">
+      <c r="V2">
+        <v>0.08599999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -632,8 +641,11 @@
       <c r="U3">
         <v>84.63934810951753</v>
       </c>
-    </row>
-    <row r="4" spans="1:21">
+      <c r="V3">
+        <v>0.102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -697,8 +709,11 @@
       <c r="U4">
         <v>75.21077821011671</v>
       </c>
-    </row>
-    <row r="5" spans="1:21">
+      <c r="V4">
+        <v>0.107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -762,24 +777,33 @@
       <c r="U5">
         <v>88.11775193798438</v>
       </c>
-    </row>
-    <row r="6" spans="1:21">
+      <c r="V5">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>41122.16666666666</v>
       </c>
-    </row>
-    <row r="7" spans="1:21">
+      <c r="V6">
+        <v>0.129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>41152.58333333334</v>
       </c>
-    </row>
-    <row r="8" spans="1:21">
+      <c r="V7">
+        <v>0.232</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -787,63 +811,84 @@
         <v>41183</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:22">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>41213.41666666666</v>
       </c>
-    </row>
-    <row r="10" spans="1:21">
+      <c r="V9">
+        <v>0.154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>41243.83333333334</v>
       </c>
-    </row>
-    <row r="11" spans="1:21">
+      <c r="V10">
+        <v>0.177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>41274.25</v>
       </c>
-    </row>
-    <row r="12" spans="1:21">
+      <c r="V11">
+        <v>0.188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>41304.66666666666</v>
       </c>
-    </row>
-    <row r="13" spans="1:21">
+      <c r="V12">
+        <v>0.192</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>41335.08333333334</v>
       </c>
-    </row>
-    <row r="14" spans="1:21">
+      <c r="V13">
+        <v>0.182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" s="2">
         <v>41365.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:21">
+      <c r="V14">
+        <v>0.265</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" s="2">
         <v>41395.91666666666</v>
       </c>
-    </row>
-    <row r="16" spans="1:21">
+      <c r="V15">
+        <v>0.266</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -851,31 +896,40 @@
         <v>41426.33333333334</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:22">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" s="2">
         <v>41456.75</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="V17">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" s="2">
         <v>41487.16666666666</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="V18">
+        <v>0.273</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>41517.58333333334</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="V19">
+        <v>0.124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -883,7 +937,7 @@
         <v>41548</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:22">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -891,7 +945,7 @@
         <v>41578.41666666666</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:22">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -899,7 +953,7 @@
         <v>41608.83333333334</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:22">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -907,7 +961,7 @@
         <v>41639.25</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:22">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -915,7 +969,7 @@
         <v>41669.66666666666</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:22">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -923,15 +977,18 @@
         <v>41700.08333333334</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:22">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" s="2">
         <v>41730.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="V26">
+        <v>0.232</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -939,7 +996,7 @@
         <v>41760.91666666666</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:22">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -947,7 +1004,7 @@
         <v>41791.33333333334</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:22">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -955,7 +1012,7 @@
         <v>41821.75</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:22">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -963,7 +1020,7 @@
         <v>41852.16666666666</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:22">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -971,7 +1028,7 @@
         <v>41882.58333333334</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:22">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -979,7 +1036,7 @@
         <v>41913</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:22">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -987,7 +1044,7 @@
         <v>41943.41666666666</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:22">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -995,31 +1052,40 @@
         <v>41973.83333333334</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:22">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" s="2">
         <v>42004.25</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="V35">
+        <v>0.215</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" s="2">
         <v>42034.66666666666</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="V36">
+        <v>0.195</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" s="2">
         <v>42065.08333333334</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="V37">
+        <v>0.204</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1027,7 +1093,7 @@
         <v>42095.5</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:22">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1035,7 +1101,7 @@
         <v>42125.91666666666</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:22">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1043,15 +1109,18 @@
         <v>42156.33333333334</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:22">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" s="2">
         <v>42186.75</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="V41">
+        <v>0.467</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1059,23 +1128,29 @@
         <v>42217.16666666666</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:22">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" s="2">
         <v>42247.58333333334</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="V43">
+        <v>0.205</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" s="2">
         <v>42278</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="V44">
+        <v>0.283</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1083,23 +1158,29 @@
         <v>42308.41666666666</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:22">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46" s="2">
         <v>42338.83333333334</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="V46">
+        <v>0.265</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" s="2">
         <v>42369.25</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="V47">
+        <v>0.2645</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1107,7 +1188,7 @@
         <v>42399.66666666666</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:22">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1115,7 +1196,7 @@
         <v>42430.08333333334</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:22">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1123,23 +1204,29 @@
         <v>42460.5</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:22">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51" s="2">
         <v>42490.91666666666</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="V51">
+        <v>0.2383333333333333</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22">
       <c r="A52" s="1">
         <v>50</v>
       </c>
       <c r="B52" s="2">
         <v>42521.33333333334</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="V52">
+        <v>0.193</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1147,7 +1234,7 @@
         <v>42551.75</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:22">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1155,15 +1242,18 @@
         <v>42582.16666666666</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:22">
       <c r="A55" s="1">
         <v>53</v>
       </c>
       <c r="B55" s="2">
         <v>42612.58333333334</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="V55">
+        <v>0.179</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -1171,7 +1261,7 @@
         <v>42643</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:22">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -1179,7 +1269,7 @@
         <v>42673.41666666666</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:22">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -1187,23 +1277,29 @@
         <v>42703.83333333334</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:22">
       <c r="A59" s="1">
         <v>57</v>
       </c>
       <c r="B59" s="2">
         <v>42734.25</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
+      <c r="V59">
+        <v>0.274</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22">
       <c r="A60" s="1">
         <v>58</v>
       </c>
       <c r="B60" s="2">
         <v>42764.66666666666</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
+      <c r="V60">
+        <v>0.209</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -1211,55 +1307,73 @@
         <v>42795.08333333334</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:22">
       <c r="A62" s="1">
         <v>60</v>
       </c>
       <c r="B62" s="2">
         <v>42825.5</v>
       </c>
-    </row>
-    <row r="63" spans="1:2">
+      <c r="V62">
+        <v>0.293</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22">
       <c r="A63" s="1">
         <v>61</v>
       </c>
       <c r="B63" s="2">
         <v>42855.91666666666</v>
       </c>
-    </row>
-    <row r="64" spans="1:2">
+      <c r="V63">
+        <v>0.238</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22">
       <c r="A64" s="1">
         <v>62</v>
       </c>
       <c r="B64" s="2">
         <v>42886.33333333334</v>
       </c>
-    </row>
-    <row r="65" spans="1:2">
+      <c r="V64">
+        <v>0.416</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22">
       <c r="A65" s="1">
         <v>63</v>
       </c>
       <c r="B65" s="2">
         <v>42916.75</v>
       </c>
-    </row>
-    <row r="66" spans="1:2">
+      <c r="V65">
+        <v>0.4625</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22">
       <c r="A66" s="1">
         <v>64</v>
       </c>
       <c r="B66" s="2">
         <v>42947.16666666666</v>
       </c>
-    </row>
-    <row r="67" spans="1:2">
+      <c r="V66">
+        <v>0.606</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22">
       <c r="A67" s="1">
         <v>65</v>
       </c>
       <c r="B67" s="2">
         <v>42977.58333333334</v>
       </c>
-    </row>
-    <row r="68" spans="1:2">
+      <c r="V67">
+        <v>0.5628461538461539</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -1267,7 +1381,7 @@
         <v>43008</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:22">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -1275,15 +1389,18 @@
         <v>43038.41666666666</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:22">
       <c r="A70" s="1">
         <v>68</v>
       </c>
       <c r="B70" s="2">
         <v>43068.83333333334</v>
       </c>
-    </row>
-    <row r="71" spans="1:2">
+      <c r="V70">
+        <v>0.322</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -1291,7 +1408,7 @@
         <v>43099.25</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:22">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -1299,7 +1416,7 @@
         <v>43129.66666666666</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:22">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -1307,15 +1424,18 @@
         <v>43160.08333333334</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:22">
       <c r="A74" s="1">
         <v>72</v>
       </c>
       <c r="B74" s="2">
         <v>43190.5</v>
       </c>
-    </row>
-    <row r="75" spans="1:2">
+      <c r="V74">
+        <v>0.2132</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -1323,39 +1443,51 @@
         <v>43220.91666666666</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:22">
       <c r="A76" s="1">
         <v>74</v>
       </c>
       <c r="B76" s="2">
         <v>43251.33333333334</v>
       </c>
-    </row>
-    <row r="77" spans="1:2">
+      <c r="V76">
+        <v>0.2825</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22">
       <c r="A77" s="1">
         <v>75</v>
       </c>
       <c r="B77" s="2">
         <v>43281.75</v>
       </c>
-    </row>
-    <row r="78" spans="1:2">
+      <c r="V77">
+        <v>0.2700909090909091</v>
+      </c>
+    </row>
+    <row r="78" spans="1:22">
       <c r="A78" s="1">
         <v>76</v>
       </c>
       <c r="B78" s="2">
         <v>43312.16666666666</v>
       </c>
-    </row>
-    <row r="79" spans="1:2">
+      <c r="V78">
+        <v>0.2696</v>
+      </c>
+    </row>
+    <row r="79" spans="1:22">
       <c r="A79" s="1">
         <v>77</v>
       </c>
       <c r="B79" s="2">
         <v>43342.58333333334</v>
       </c>
-    </row>
-    <row r="80" spans="1:2">
+      <c r="V79">
+        <v>0.2712</v>
+      </c>
+    </row>
+    <row r="80" spans="1:22">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -1363,31 +1495,40 @@
         <v>43373</v>
       </c>
     </row>
-    <row r="81" spans="1:21">
+    <row r="81" spans="1:22">
       <c r="A81" s="1">
         <v>79</v>
       </c>
       <c r="B81" s="2">
         <v>43403.41666666666</v>
       </c>
-    </row>
-    <row r="82" spans="1:21">
+      <c r="V81">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="82" spans="1:22">
       <c r="A82" s="1">
         <v>80</v>
       </c>
       <c r="B82" s="2">
         <v>43433.83333333334</v>
       </c>
-    </row>
-    <row r="83" spans="1:21">
+      <c r="V82">
+        <v>0.359</v>
+      </c>
+    </row>
+    <row r="83" spans="1:22">
       <c r="A83" s="1">
         <v>81</v>
       </c>
       <c r="B83" s="2">
         <v>43464.25</v>
       </c>
-    </row>
-    <row r="84" spans="1:21">
+      <c r="V83">
+        <v>0.272</v>
+      </c>
+    </row>
+    <row r="84" spans="1:22">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -1395,7 +1536,7 @@
         <v>43494.66666666666</v>
       </c>
     </row>
-    <row r="85" spans="1:21">
+    <row r="85" spans="1:22">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -1403,7 +1544,7 @@
         <v>43525.08333333334</v>
       </c>
     </row>
-    <row r="86" spans="1:21">
+    <row r="86" spans="1:22">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -1411,15 +1552,18 @@
         <v>43555.5</v>
       </c>
     </row>
-    <row r="87" spans="1:21">
+    <row r="87" spans="1:22">
       <c r="A87" s="1">
         <v>85</v>
       </c>
       <c r="B87" s="2">
         <v>43585.91666666666</v>
       </c>
-    </row>
-    <row r="88" spans="1:21">
+      <c r="V87">
+        <v>0.328</v>
+      </c>
+    </row>
+    <row r="88" spans="1:22">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -1427,39 +1571,51 @@
         <v>43616.33333333334</v>
       </c>
     </row>
-    <row r="89" spans="1:21">
+    <row r="89" spans="1:22">
       <c r="A89" s="1">
         <v>87</v>
       </c>
       <c r="B89" s="2">
         <v>43646.75</v>
       </c>
-    </row>
-    <row r="90" spans="1:21">
+      <c r="V89">
+        <v>0.216</v>
+      </c>
+    </row>
+    <row r="90" spans="1:22">
       <c r="A90" s="1">
         <v>88</v>
       </c>
       <c r="B90" s="2">
         <v>43677.16666666666</v>
       </c>
-    </row>
-    <row r="91" spans="1:21">
+      <c r="V90">
+        <v>0.3143333333333334</v>
+      </c>
+    </row>
+    <row r="91" spans="1:22">
       <c r="A91" s="1">
         <v>89</v>
       </c>
       <c r="B91" s="2">
         <v>43707.58333333334</v>
       </c>
-    </row>
-    <row r="92" spans="1:21">
+      <c r="V91">
+        <v>0.236</v>
+      </c>
+    </row>
+    <row r="92" spans="1:22">
       <c r="A92" s="1">
         <v>90</v>
       </c>
       <c r="B92" s="2">
         <v>43738</v>
       </c>
-    </row>
-    <row r="93" spans="1:21">
+      <c r="V92">
+        <v>0.495875</v>
+      </c>
+    </row>
+    <row r="93" spans="1:22">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -1523,8 +1679,11 @@
       <c r="U93">
         <v>81.98936936936931</v>
       </c>
-    </row>
-    <row r="94" spans="1:21">
+      <c r="V93">
+        <v>0.123</v>
+      </c>
+    </row>
+    <row r="94" spans="1:22">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -1588,8 +1747,11 @@
       <c r="U94">
         <v>80.98093264248699</v>
       </c>
-    </row>
-    <row r="95" spans="1:21">
+      <c r="V94">
+        <v>0.42675</v>
+      </c>
+    </row>
+    <row r="95" spans="1:22">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -1597,23 +1759,29 @@
         <v>43829.25</v>
       </c>
     </row>
-    <row r="96" spans="1:21">
+    <row r="96" spans="1:22">
       <c r="A96" s="1">
         <v>94</v>
       </c>
       <c r="B96" s="2">
         <v>43859.66666666666</v>
       </c>
-    </row>
-    <row r="97" spans="1:21">
+      <c r="V96">
+        <v>0.11475</v>
+      </c>
+    </row>
+    <row r="97" spans="1:22">
       <c r="A97" s="1">
         <v>95</v>
       </c>
       <c r="B97" s="2">
         <v>43890.08333333334</v>
       </c>
-    </row>
-    <row r="98" spans="1:21">
+      <c r="V97">
+        <v>0.1083333333333333</v>
+      </c>
+    </row>
+    <row r="98" spans="1:22">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -1677,8 +1845,11 @@
       <c r="U98">
         <v>52.66595690747781</v>
       </c>
-    </row>
-    <row r="99" spans="1:21">
+      <c r="V98">
+        <v>0.305</v>
+      </c>
+    </row>
+    <row r="99" spans="1:22">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -1742,8 +1913,11 @@
       <c r="U99">
         <v>52.7998081841432</v>
       </c>
-    </row>
-    <row r="100" spans="1:21">
+      <c r="V99">
+        <v>0.399909090909091</v>
+      </c>
+    </row>
+    <row r="100" spans="1:22">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -1807,8 +1981,11 @@
       <c r="U100">
         <v>52.79993564993563</v>
       </c>
-    </row>
-    <row r="101" spans="1:21">
+      <c r="V100">
+        <v>0.3882307692307693</v>
+      </c>
+    </row>
+    <row r="101" spans="1:22">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -1816,7 +1993,7 @@
         <v>44011.75</v>
       </c>
     </row>
-    <row r="102" spans="1:21">
+    <row r="102" spans="1:22">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -1824,7 +2001,7 @@
         <v>44042.16666666666</v>
       </c>
     </row>
-    <row r="103" spans="1:21">
+    <row r="103" spans="1:22">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -1832,7 +2009,7 @@
         <v>44072.58333333334</v>
       </c>
     </row>
-    <row r="104" spans="1:21">
+    <row r="104" spans="1:22">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -1840,7 +2017,7 @@
         <v>44103</v>
       </c>
     </row>
-    <row r="105" spans="1:21">
+    <row r="105" spans="1:22">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -1848,7 +2025,7 @@
         <v>44133.41666666666</v>
       </c>
     </row>
-    <row r="106" spans="1:21">
+    <row r="106" spans="1:22">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -1856,7 +2033,7 @@
         <v>44163.83333333334</v>
       </c>
     </row>
-    <row r="107" spans="1:21">
+    <row r="107" spans="1:22">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -1864,7 +2041,7 @@
         <v>44194.25</v>
       </c>
     </row>
-    <row r="108" spans="1:21">
+    <row r="108" spans="1:22">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -1872,7 +2049,7 @@
         <v>44224.66666666666</v>
       </c>
     </row>
-    <row r="109" spans="1:21">
+    <row r="109" spans="1:22">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -1880,17 +2057,17 @@
         <v>44255.08333333334</v>
       </c>
     </row>
-    <row r="110" spans="1:21">
+    <row r="110" spans="1:22">
       <c r="A110" s="1">
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:21">
+    <row r="111" spans="1:22">
       <c r="A111" s="1">
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:21">
+    <row r="112" spans="1:22">
       <c r="A112" s="1">
         <v>110</v>
       </c>

</xml_diff>